<commit_message>
Update before adding Eskom data
</commit_message>
<xml_diff>
--- a/data/Existing Power Stations SA.xlsx
+++ b/data/Existing Power Stations SA.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pypsa-za\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61CA91F-7688-42E8-BC5B-D6A7A695EBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10678FA-678C-42E6-93C1-D2913DAC4D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -444,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,9 +477,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -850,9 +847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H74" sqref="H74"/>
+      <selection pane="topRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,7 +887,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>111</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -991,8 +988,8 @@
       <c r="J2" s="6">
         <v>11.654</v>
       </c>
-      <c r="K2" s="12">
-        <v>26</v>
+      <c r="K2" s="6">
+        <v>16.8</v>
       </c>
       <c r="L2" s="6">
         <v>2.1</v>
@@ -1000,7 +997,7 @@
       <c r="M2" s="6">
         <v>2.1</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="13">
         <v>0.5</v>
       </c>
       <c r="O2" s="6">
@@ -1074,8 +1071,8 @@
       <c r="J3" s="6">
         <v>12.420999999999999</v>
       </c>
-      <c r="K3" s="12">
-        <v>26</v>
+      <c r="K3" s="6">
+        <v>23.1</v>
       </c>
       <c r="L3" s="6">
         <v>1.1000000000000001</v>
@@ -1083,7 +1080,7 @@
       <c r="M3" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="13">
         <v>0.5</v>
       </c>
       <c r="O3" s="6">
@@ -1157,8 +1154,8 @@
       <c r="J4" s="6">
         <v>11.034000000000001</v>
       </c>
-      <c r="K4" s="12">
-        <v>26</v>
+      <c r="K4" s="6">
+        <v>11.8</v>
       </c>
       <c r="L4" s="6">
         <v>3.3</v>
@@ -1166,7 +1163,7 @@
       <c r="M4" s="6">
         <v>3.3</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="13">
         <v>0.5</v>
       </c>
       <c r="O4" s="6">
@@ -1240,8 +1237,8 @@
       <c r="J5" s="6">
         <v>12.61</v>
       </c>
-      <c r="K5" s="12">
-        <v>26</v>
+      <c r="K5" s="6">
+        <v>22.1</v>
       </c>
       <c r="L5" s="6">
         <v>0.9</v>
@@ -1249,7 +1246,7 @@
       <c r="M5" s="6">
         <v>0.9</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="13">
         <v>0.5</v>
       </c>
       <c r="O5" s="6">
@@ -1317,14 +1314,14 @@
         <v>10</v>
       </c>
       <c r="H6" s="9"/>
-      <c r="I6" s="16">
+      <c r="I6" s="15">
         <v>46023</v>
       </c>
       <c r="J6" s="6">
         <v>12.131</v>
       </c>
-      <c r="K6" s="12">
-        <v>26</v>
+      <c r="K6" s="6">
+        <v>17</v>
       </c>
       <c r="L6" s="6">
         <v>1.1000000000000001</v>
@@ -1332,7 +1329,7 @@
       <c r="M6" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="13">
         <v>0.5</v>
       </c>
       <c r="O6" s="6">
@@ -1400,14 +1397,14 @@
         <v>6</v>
       </c>
       <c r="H7" s="9"/>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <v>52232</v>
       </c>
       <c r="J7" s="6">
         <v>11.753</v>
       </c>
-      <c r="K7" s="12">
-        <v>26</v>
+      <c r="K7" s="6">
+        <v>18.600000000000001</v>
       </c>
       <c r="L7" s="6">
         <v>1.8</v>
@@ -1415,7 +1412,7 @@
       <c r="M7" s="6">
         <v>1.8</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="13">
         <v>0.5</v>
       </c>
       <c r="O7" s="6">
@@ -1483,14 +1480,14 @@
         <v>9</v>
       </c>
       <c r="H8" s="9"/>
-      <c r="I8" s="16">
+      <c r="I8" s="15">
         <v>46753</v>
       </c>
       <c r="J8" s="6">
         <v>13.829000000000001</v>
       </c>
-      <c r="K8" s="12">
-        <v>26</v>
+      <c r="K8" s="6">
+        <v>17.600000000000001</v>
       </c>
       <c r="L8" s="6">
         <v>0.5</v>
@@ -1498,7 +1495,7 @@
       <c r="M8" s="6">
         <v>0.5</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="13">
         <v>0.5</v>
       </c>
       <c r="O8" s="6">
@@ -1566,14 +1563,14 @@
         <v>6</v>
       </c>
       <c r="H9" s="9"/>
-      <c r="I9" s="16">
+      <c r="I9" s="15">
         <v>47119</v>
       </c>
       <c r="J9" s="6">
         <v>11.243</v>
       </c>
-      <c r="K9" s="12">
-        <v>26</v>
+      <c r="K9" s="6">
+        <v>18.600000000000001</v>
       </c>
       <c r="L9" s="6">
         <v>3.6</v>
@@ -1581,7 +1578,7 @@
       <c r="M9" s="6">
         <v>3.6</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="13">
         <v>0.5</v>
       </c>
       <c r="O9" s="6">
@@ -1651,14 +1648,14 @@
       <c r="H10" s="9">
         <v>45658</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>96</v>
       </c>
       <c r="J10" s="6">
         <v>9.8119999999999994</v>
       </c>
-      <c r="K10" s="12">
-        <v>26</v>
+      <c r="K10" s="6">
+        <v>16.3</v>
       </c>
       <c r="L10" s="6">
         <v>7.2</v>
@@ -1666,7 +1663,7 @@
       <c r="M10" s="6">
         <v>7.2</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="13">
         <v>0.5</v>
       </c>
       <c r="O10" s="6">
@@ -1734,14 +1731,14 @@
         <v>6</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="16">
+      <c r="I11" s="15">
         <v>51136</v>
       </c>
       <c r="J11" s="6">
         <v>10.975</v>
       </c>
-      <c r="K11" s="12">
-        <v>26</v>
+      <c r="K11" s="6">
+        <v>11.2</v>
       </c>
       <c r="L11" s="6">
         <v>5.9</v>
@@ -1749,7 +1746,7 @@
       <c r="M11" s="6">
         <v>5.9</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="13">
         <v>0.5</v>
       </c>
       <c r="O11" s="6">
@@ -1817,14 +1814,14 @@
         <v>3</v>
       </c>
       <c r="H12" s="9"/>
-      <c r="I12" s="16">
+      <c r="I12" s="15">
         <v>54058</v>
       </c>
       <c r="J12" s="6">
         <v>11.753</v>
       </c>
-      <c r="K12" s="12">
-        <v>26</v>
+      <c r="K12" s="6">
+        <v>21.8</v>
       </c>
       <c r="L12" s="6">
         <v>1.7</v>
@@ -1832,7 +1829,7 @@
       <c r="M12" s="6">
         <v>1.7</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="13">
         <v>0.5</v>
       </c>
       <c r="O12" s="6">
@@ -1900,14 +1897,14 @@
         <v>3</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="16">
+      <c r="I13" s="15">
         <v>55154</v>
       </c>
       <c r="J13" s="6">
         <v>11.004</v>
       </c>
-      <c r="K13" s="12">
-        <v>26</v>
+      <c r="K13" s="6">
+        <v>23.3</v>
       </c>
       <c r="L13" s="6">
         <v>1.9</v>
@@ -1915,7 +1912,7 @@
       <c r="M13" s="6">
         <v>1.9</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="13">
         <v>0.5</v>
       </c>
       <c r="O13" s="6">
@@ -1983,14 +1980,14 @@
         <v>6</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="I14" s="16">
+      <c r="I14" s="15">
         <v>51502</v>
       </c>
       <c r="J14" s="6">
         <v>11.654</v>
       </c>
-      <c r="K14" s="12">
-        <v>26</v>
+      <c r="K14" s="6">
+        <v>11.4</v>
       </c>
       <c r="L14" s="6">
         <v>3</v>
@@ -1998,7 +1995,7 @@
       <c r="M14" s="6">
         <v>3</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="13">
         <v>0.5</v>
       </c>
       <c r="O14" s="6">
@@ -2066,14 +2063,14 @@
         <v>6</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <v>48580</v>
       </c>
       <c r="J15" s="6">
         <v>11.034000000000001</v>
       </c>
-      <c r="K15" s="12">
-        <v>26</v>
+      <c r="K15" s="6">
+        <v>22.9</v>
       </c>
       <c r="L15" s="6">
         <v>2.4</v>
@@ -2081,7 +2078,7 @@
       <c r="M15" s="6">
         <v>2.4</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="13">
         <v>0.5</v>
       </c>
       <c r="O15" s="6">
@@ -2149,14 +2146,14 @@
         <v>1</v>
       </c>
       <c r="H16" s="9"/>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J16" s="6">
         <v>9.8119999999999994</v>
       </c>
-      <c r="K16" s="12">
-        <v>26</v>
+      <c r="K16" s="6">
+        <v>16.3</v>
       </c>
       <c r="L16" s="6">
         <v>7.2</v>
@@ -2164,7 +2161,7 @@
       <c r="M16" s="6">
         <v>7.2</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="13">
         <v>0.5</v>
       </c>
       <c r="O16" s="6">
@@ -2232,13 +2229,13 @@
         <v>6</v>
       </c>
       <c r="H17" s="9"/>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <v>51136</v>
       </c>
       <c r="J17" s="6">
         <v>10.917999999999999</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="6">
         <v>26</v>
       </c>
       <c r="L17" s="6">
@@ -2247,7 +2244,7 @@
       <c r="M17" s="6">
         <v>3.2</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="13">
         <v>0.5</v>
       </c>
       <c r="O17" s="6">
@@ -2315,7 +2312,7 @@
         <v>50</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="20">
+      <c r="I18" s="19">
         <v>49064</v>
       </c>
       <c r="J18" s="5" t="s">
@@ -2330,7 +2327,7 @@
       <c r="M18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="14">
         <v>0</v>
       </c>
       <c r="O18" s="6">
@@ -2398,7 +2395,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="19">
+      <c r="I19" s="18">
         <v>52597</v>
       </c>
       <c r="J19" s="6">
@@ -2413,7 +2410,7 @@
       <c r="M19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="14">
         <v>0</v>
       </c>
       <c r="O19" s="6">
@@ -2481,7 +2478,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="9"/>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J20" s="5" t="s">
@@ -2496,7 +2493,7 @@
       <c r="M20" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N20" s="15">
+      <c r="N20" s="14">
         <v>0</v>
       </c>
       <c r="O20" s="6">
@@ -2566,7 +2563,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J21" s="5" t="s">
@@ -2581,7 +2578,7 @@
       <c r="M21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N21" s="15">
+      <c r="N21" s="14">
         <v>0</v>
       </c>
       <c r="O21" s="6">
@@ -2651,7 +2648,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J22" s="5" t="s">
@@ -2666,7 +2663,7 @@
       <c r="M22" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N22" s="15">
+      <c r="N22" s="14">
         <v>0</v>
       </c>
       <c r="O22" s="6">
@@ -2736,7 +2733,7 @@
         <v>4</v>
       </c>
       <c r="H23" s="9"/>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J23" s="5" t="s">
@@ -2751,7 +2748,7 @@
       <c r="M23" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N23" s="15">
+      <c r="N23" s="14">
         <v>0</v>
       </c>
       <c r="O23" s="6">
@@ -2819,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J24" s="5" t="s">
@@ -2834,7 +2831,7 @@
       <c r="M24" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N24" s="15">
+      <c r="N24" s="14">
         <v>0</v>
       </c>
       <c r="O24" s="6">
@@ -2902,7 +2899,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="9"/>
-      <c r="I25" s="21">
+      <c r="I25" s="20">
         <v>46022</v>
       </c>
       <c r="J25" s="6">
@@ -2917,7 +2914,7 @@
       <c r="M25" s="6">
         <v>3.4</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="14">
         <v>0</v>
       </c>
       <c r="O25" s="6">
@@ -2985,7 +2982,7 @@
         <v>9</v>
       </c>
       <c r="H26" s="9"/>
-      <c r="I26" s="21">
+      <c r="I26" s="20">
         <v>50040</v>
       </c>
       <c r="J26" s="6">
@@ -3000,7 +2997,7 @@
       <c r="M26" s="6">
         <v>9</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N26" s="14">
         <v>0</v>
       </c>
       <c r="O26" s="6">
@@ -3068,7 +3065,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="9"/>
-      <c r="I27" s="21">
+      <c r="I27" s="20">
         <v>50040</v>
       </c>
       <c r="J27" s="6">
@@ -3083,7 +3080,7 @@
       <c r="M27" s="6">
         <v>9</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="14">
         <v>0</v>
       </c>
       <c r="O27" s="6">
@@ -3151,7 +3148,7 @@
         <v>3</v>
       </c>
       <c r="H28" s="9"/>
-      <c r="I28" s="21">
+      <c r="I28" s="20">
         <v>46022</v>
       </c>
       <c r="J28" s="6">
@@ -3166,7 +3163,7 @@
       <c r="M28" s="6">
         <v>3.4</v>
       </c>
-      <c r="N28" s="15">
+      <c r="N28" s="14">
         <v>0</v>
       </c>
       <c r="O28" s="6">
@@ -3236,7 +3233,7 @@
       <c r="H29" s="11">
         <v>46023</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I29" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J29" s="5" t="s">
@@ -3251,7 +3248,7 @@
       <c r="M29" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N29" s="15">
+      <c r="N29" s="14">
         <v>0</v>
       </c>
       <c r="O29" s="6">
@@ -3315,7 +3312,7 @@
       <c r="H30" s="11">
         <v>46023</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J30" s="5" t="s">
@@ -3330,7 +3327,7 @@
       <c r="M30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N30" s="15">
+      <c r="N30" s="14">
         <v>0</v>
       </c>
       <c r="O30" s="6">
@@ -3394,7 +3391,7 @@
       <c r="H31" s="11">
         <v>46023</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="17" t="s">
         <v>96</v>
       </c>
       <c r="J31" s="5" t="s">
@@ -3409,7 +3406,7 @@
       <c r="M31" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N31" s="15">
+      <c r="N31" s="14">
         <v>0</v>
       </c>
       <c r="O31" s="6">
@@ -3470,7 +3467,7 @@
       <c r="G32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I32" s="18" t="str">
+      <c r="I32" s="17" t="str">
         <f>I31</f>
         <v>beyond 2050</v>
       </c>
@@ -3486,7 +3483,7 @@
       <c r="M32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N32" s="15">
+      <c r="N32" s="14">
         <v>0</v>
       </c>
       <c r="O32" s="6">
@@ -3556,7 +3553,7 @@
       <c r="H33" s="11">
         <v>46023</v>
       </c>
-      <c r="I33" s="18" t="str">
+      <c r="I33" s="17" t="str">
         <f t="shared" ref="I33:I47" si="2">I32</f>
         <v>beyond 2050</v>
       </c>
@@ -3572,7 +3569,7 @@
       <c r="M33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N33" s="15">
+      <c r="N33" s="14">
         <v>0</v>
       </c>
       <c r="O33" s="6">
@@ -3642,7 +3639,7 @@
       <c r="H34" s="11">
         <v>46023</v>
       </c>
-      <c r="I34" s="18" t="str">
+      <c r="I34" s="17" t="str">
         <f t="shared" si="2"/>
         <v>beyond 2050</v>
       </c>
@@ -3658,7 +3655,7 @@
       <c r="M34" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N34" s="15">
+      <c r="N34" s="14">
         <v>0</v>
       </c>
       <c r="O34" s="6">
@@ -3719,7 +3716,7 @@
       <c r="G35" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I35" s="18" t="str">
+      <c r="I35" s="17" t="str">
         <f t="shared" si="2"/>
         <v>beyond 2050</v>
       </c>
@@ -3735,7 +3732,7 @@
       <c r="M35" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N35" s="15">
+      <c r="N35" s="14">
         <v>0</v>
       </c>
       <c r="O35" s="6">
@@ -3802,7 +3799,7 @@
       <c r="G36" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I36" s="18" t="str">
+      <c r="I36" s="17" t="str">
         <f t="shared" si="2"/>
         <v>beyond 2050</v>
       </c>
@@ -3818,7 +3815,7 @@
       <c r="M36" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N36" s="15">
+      <c r="N36" s="14">
         <v>0</v>
       </c>
       <c r="O36" s="6">
@@ -3904,7 +3901,7 @@
       <c r="M37" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N37" s="15">
+      <c r="N37" s="14">
         <v>0</v>
       </c>
       <c r="O37" s="6">
@@ -3984,7 +3981,7 @@
       <c r="M38" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N38" s="15">
+      <c r="N38" s="14">
         <v>0</v>
       </c>
       <c r="O38" s="6">
@@ -4061,7 +4058,7 @@
       <c r="M39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N39" s="15">
+      <c r="N39" s="14">
         <v>0</v>
       </c>
       <c r="O39" s="6">
@@ -4138,7 +4135,7 @@
       <c r="M40" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N40" s="15">
+      <c r="N40" s="14">
         <v>0</v>
       </c>
       <c r="O40" s="6">
@@ -4218,7 +4215,7 @@
       <c r="M41" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N41" s="15">
+      <c r="N41" s="14">
         <v>0</v>
       </c>
       <c r="O41" s="6">
@@ -4295,7 +4292,7 @@
       <c r="M42" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N42" s="15">
+      <c r="N42" s="14">
         <v>0</v>
       </c>
       <c r="O42" s="6">
@@ -4372,7 +4369,7 @@
       <c r="M43" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N43" s="15">
+      <c r="N43" s="14">
         <v>0</v>
       </c>
       <c r="O43" s="6">
@@ -4449,7 +4446,7 @@
       <c r="M44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N44" s="15">
+      <c r="N44" s="14">
         <v>0</v>
       </c>
       <c r="O44" s="6">
@@ -4529,7 +4526,7 @@
       <c r="M45" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N45" s="15">
+      <c r="N45" s="14">
         <v>0</v>
       </c>
       <c r="O45" s="6">
@@ -4609,7 +4606,7 @@
       <c r="M46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N46" s="15">
+      <c r="N46" s="14">
         <v>0</v>
       </c>
       <c r="O46" s="6">
@@ -4689,7 +4686,7 @@
       <c r="M47" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N47" s="15">
+      <c r="N47" s="14">
         <v>0</v>
       </c>
       <c r="O47" s="6">
@@ -4765,7 +4762,7 @@
       <c r="M48" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N48" s="15">
+      <c r="N48" s="14">
         <v>0</v>
       </c>
       <c r="O48" s="6">
@@ -4845,7 +4842,7 @@
       <c r="M49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N49" s="15">
+      <c r="N49" s="14">
         <v>0</v>
       </c>
       <c r="O49" s="6">
@@ -4925,7 +4922,7 @@
       <c r="M50" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N50" s="15">
+      <c r="N50" s="14">
         <v>0</v>
       </c>
       <c r="O50" s="6">
@@ -5002,7 +4999,7 @@
       <c r="M51" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N51" s="15">
+      <c r="N51" s="14">
         <v>0</v>
       </c>
       <c r="O51" s="6">
@@ -5079,7 +5076,7 @@
       <c r="M52" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N52" s="15">
+      <c r="N52" s="14">
         <v>0</v>
       </c>
       <c r="O52" s="6">
@@ -5156,7 +5153,7 @@
       <c r="M53" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N53" s="15">
+      <c r="N53" s="14">
         <v>0</v>
       </c>
       <c r="O53" s="6">
@@ -5236,7 +5233,7 @@
       <c r="M54" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N54" s="15">
+      <c r="N54" s="14">
         <v>0</v>
       </c>
       <c r="O54" s="6">
@@ -5316,7 +5313,7 @@
       <c r="M55" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N55" s="15">
+      <c r="N55" s="14">
         <v>0</v>
       </c>
       <c r="O55" s="6">
@@ -5396,7 +5393,7 @@
       <c r="M56" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N56" s="15">
+      <c r="N56" s="14">
         <v>0</v>
       </c>
       <c r="O56" s="6">
@@ -5476,7 +5473,7 @@
       <c r="M57" s="6">
         <v>3.06</v>
       </c>
-      <c r="N57" s="14">
+      <c r="N57" s="13">
         <v>0.5</v>
       </c>
       <c r="O57" s="6">
@@ -5556,7 +5553,7 @@
       <c r="M58" s="6">
         <v>2.7865000000000002</v>
       </c>
-      <c r="N58" s="14">
+      <c r="N58" s="13">
         <v>0.5</v>
       </c>
       <c r="O58" s="6">
@@ -5633,7 +5630,7 @@
       <c r="M59" s="6">
         <v>0.5</v>
       </c>
-      <c r="N59" s="14">
+      <c r="N59" s="13">
         <v>0.5</v>
       </c>
       <c r="O59" s="6">
@@ -5716,7 +5713,7 @@
       <c r="M60" s="6">
         <v>0.5</v>
       </c>
-      <c r="N60" s="14">
+      <c r="N60" s="13">
         <v>0.5</v>
       </c>
       <c r="O60" s="6">
@@ -5799,7 +5796,7 @@
       <c r="M61" s="6">
         <v>11</v>
       </c>
-      <c r="N61" s="15">
+      <c r="N61" s="14">
         <v>0</v>
       </c>
       <c r="O61" s="6">
@@ -5882,7 +5879,7 @@
       <c r="M62" s="6">
         <v>11</v>
       </c>
-      <c r="N62" s="15">
+      <c r="N62" s="14">
         <v>0</v>
       </c>
       <c r="O62" s="6">
@@ -5965,7 +5962,7 @@
       <c r="M63" s="6">
         <v>8</v>
       </c>
-      <c r="N63" s="15">
+      <c r="N63" s="14">
         <v>0</v>
       </c>
       <c r="O63" s="6">
@@ -6048,7 +6045,7 @@
       <c r="M64" s="6">
         <v>2</v>
       </c>
-      <c r="N64" s="15">
+      <c r="N64" s="14">
         <v>0</v>
       </c>
       <c r="O64" s="6">
@@ -6131,7 +6128,7 @@
       <c r="M65" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N65" s="15">
+      <c r="N65" s="14">
         <v>0</v>
       </c>
       <c r="O65" s="6">
@@ -6208,7 +6205,7 @@
       <c r="M66" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N66" s="15">
+      <c r="N66" s="14">
         <v>0</v>
       </c>
       <c r="O66" s="6">
@@ -6291,7 +6288,7 @@
       <c r="M67" s="6">
         <v>0.5</v>
       </c>
-      <c r="N67" s="15">
+      <c r="N67" s="14">
         <v>0</v>
       </c>
       <c r="O67" s="6">
@@ -6368,7 +6365,7 @@
       <c r="M68" s="6">
         <v>0.5</v>
       </c>
-      <c r="N68" s="15">
+      <c r="N68" s="14">
         <v>0</v>
       </c>
       <c r="O68" s="6">
@@ -6451,7 +6448,7 @@
       <c r="M69" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N69" s="15">
+      <c r="N69" s="14">
         <v>0</v>
       </c>
       <c r="O69" s="6">

</xml_diff>